<commit_message>
lib: fix to .mov outputs for OSX10.5 (introduced by creating support for 10.6!)
minor fixes to tests for openpyxl

git-svn-id: https://psychopy.googlecode.com/svn/trunk@1085 1c617f74-e3c1-11dd-95e1-755cbddbdd66
</commit_message>
<xml_diff>
--- a/psychopy/tests/testData/data.xlsx
+++ b/psychopy/tests/testData/data.xlsx
@@ -91,8 +91,9 @@
 </sst>
 </file>
 
-<file path=xl/style.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -120,17 +121,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -482,10 +482,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -515,10 +515,10 @@
         <v>0.710916996002</v>
       </c>
       <c r="M2" t="n">
-        <v>0.685897</v>
+        <v>0.685896873474</v>
       </c>
       <c r="N2" t="n">
-        <v>0.735937</v>
+        <v>0.73593711853</v>
       </c>
       <c r="O2" t="n">
         <v>0.0250201225281</v>
@@ -529,10 +529,10 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -562,10 +562,10 @@
         <v>0.902688503265</v>
       </c>
       <c r="M3" t="n">
-        <v>1.03579</v>
+        <v>1.0357940197</v>
       </c>
       <c r="N3" t="n">
-        <v>0.769583</v>
+        <v>0.769582986832</v>
       </c>
       <c r="O3" t="n">
         <v>0.133105516434</v>
@@ -576,10 +576,10 @@
         <v>18</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -609,10 +609,10 @@
         <v>0.74442243576</v>
       </c>
       <c r="M4" t="n">
-        <v>0.736332</v>
+        <v>0.736331939697</v>
       </c>
       <c r="N4" t="n">
-        <v>0.752513</v>
+        <v>0.752512931824</v>
       </c>
       <c r="O4" t="n">
         <v>0.00809049606323</v>
@@ -623,10 +623,10 @@
         <v>18</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -656,10 +656,10 @@
         <v>0.74411046505</v>
       </c>
       <c r="M5" t="n">
-        <v>0.735621</v>
+        <v>0.735620975494</v>
       </c>
       <c r="N5" t="n">
-        <v>0.7526</v>
+        <v>0.752599954605</v>
       </c>
       <c r="O5" t="n">
         <v>0.00848948955536</v>
@@ -670,10 +670,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -703,10 +703,10 @@
         <v>0.602207064629</v>
       </c>
       <c r="M6" t="n">
-        <v>0.56877</v>
+        <v>0.568769931793</v>
       </c>
       <c r="N6" t="n">
-        <v>0.635644</v>
+        <v>0.635644197464</v>
       </c>
       <c r="O6" t="n">
         <v>0.0334371328354</v>
@@ -717,10 +717,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -750,10 +750,10 @@
         <v>0.727305054665</v>
       </c>
       <c r="M7" t="n">
-        <v>0.70213</v>
+        <v>0.702130079269</v>
       </c>
       <c r="N7" t="n">
-        <v>0.75248</v>
+        <v>0.75248003006</v>
       </c>
       <c r="O7" t="n">
         <v>0.0251749753952</v>
@@ -793,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="n">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>